<commit_message>
update codelist after release
</commit_message>
<xml_diff>
--- a/Codelists/Codelists - Import.xlsx
+++ b/Codelists/Codelists - Import.xlsx
@@ -1186,7 +1186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2291,12 +2291,12 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>KPW</t>
+          <t>KMF</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>North Korean Won</t>
+          <t>KMF</t>
         </is>
       </c>
       <c r="C79" s="3" t="n"/>
@@ -2305,12 +2305,12 @@
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>KRW</t>
+          <t>KPW</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>Won</t>
+          <t>North Korean Won</t>
         </is>
       </c>
       <c r="C80" s="2" t="n"/>
@@ -2319,12 +2319,12 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>KWD</t>
+          <t>KRW</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Kuwaiti Dinar</t>
+          <t>Won</t>
         </is>
       </c>
       <c r="C81" s="3" t="n"/>
@@ -2333,12 +2333,12 @@
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>KYD</t>
+          <t>KWD</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>Cayman Islands Dollar</t>
+          <t>Kuwaiti Dinar</t>
         </is>
       </c>
       <c r="C82" s="2" t="n"/>
@@ -2347,12 +2347,12 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>KZT</t>
+          <t>KYD</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Tenge</t>
+          <t>Cayman Islands Dollar</t>
         </is>
       </c>
       <c r="C83" s="3" t="n"/>
@@ -2361,12 +2361,12 @@
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>LAK</t>
+          <t>KZT</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>Lao Kip</t>
+          <t>Tenge</t>
         </is>
       </c>
       <c r="C84" s="2" t="n"/>
@@ -2375,12 +2375,12 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>LBP</t>
+          <t>LAK</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Lebanese Pound</t>
+          <t>Lao Kip</t>
         </is>
       </c>
       <c r="C85" s="3" t="n"/>
@@ -2389,12 +2389,12 @@
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>LKR</t>
+          <t>LBP</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>Sri Lanka Rupee</t>
+          <t>Lebanese Pound</t>
         </is>
       </c>
       <c r="C86" s="2" t="n"/>
@@ -2403,12 +2403,12 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>LRD</t>
+          <t>LKR</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Liberian Dollar</t>
+          <t>Sri Lanka Rupee</t>
         </is>
       </c>
       <c r="C87" s="3" t="n"/>
@@ -2417,12 +2417,12 @@
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>LSL</t>
+          <t>LRD</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>Loti</t>
+          <t>Liberian Dollar</t>
         </is>
       </c>
       <c r="C88" s="2" t="n"/>
@@ -2431,12 +2431,12 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>LYD</t>
+          <t>LSL</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Libyan Dinar</t>
+          <t>Loti</t>
         </is>
       </c>
       <c r="C89" s="3" t="n"/>
@@ -2445,12 +2445,12 @@
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MAD</t>
+          <t>LYD</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>Moroccan Dirham</t>
+          <t>Libyan Dinar</t>
         </is>
       </c>
       <c r="C90" s="2" t="n"/>
@@ -2459,12 +2459,12 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>MDL</t>
+          <t>MAD</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>Moldovan Leu</t>
+          <t>Moroccan Dirham</t>
         </is>
       </c>
       <c r="C91" s="3" t="n"/>
@@ -2473,12 +2473,12 @@
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>MGA</t>
+          <t>MDL</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>Malagasy Ariary</t>
+          <t>Moldovan Leu</t>
         </is>
       </c>
       <c r="C92" s="2" t="n"/>
@@ -2487,12 +2487,12 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>MKD</t>
+          <t>MGA</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>Denar</t>
+          <t>Malagasy Ariary</t>
         </is>
       </c>
       <c r="C93" s="3" t="n"/>
@@ -2501,12 +2501,12 @@
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>MMK</t>
+          <t>MKD</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>Kyat</t>
+          <t>Denar</t>
         </is>
       </c>
       <c r="C94" s="2" t="n"/>
@@ -2515,12 +2515,12 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>MNT</t>
+          <t>MMK</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>Tugrik</t>
+          <t>Kyat</t>
         </is>
       </c>
       <c r="C95" s="3" t="n"/>
@@ -2529,12 +2529,12 @@
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MOP</t>
+          <t>MNT</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>Pataca</t>
+          <t>Tugrik</t>
         </is>
       </c>
       <c r="C96" s="2" t="n"/>
@@ -2543,12 +2543,12 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>MRU</t>
+          <t>MOP</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>Ouguiya</t>
+          <t>Pataca</t>
         </is>
       </c>
       <c r="C97" s="3" t="n"/>
@@ -2557,12 +2557,12 @@
     <row r="98">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MUR</t>
+          <t>MRU</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>Mauritius Rupee</t>
+          <t>Ouguiya</t>
         </is>
       </c>
       <c r="C98" s="2" t="n"/>
@@ -2571,12 +2571,12 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>MVR</t>
+          <t>MUR</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Rufiyaa</t>
+          <t>Mauritius Rupee</t>
         </is>
       </c>
       <c r="C99" s="3" t="n"/>
@@ -2585,12 +2585,12 @@
     <row r="100">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MWK</t>
+          <t>MVR</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>Malawi Kwacha</t>
+          <t>Rufiyaa</t>
         </is>
       </c>
       <c r="C100" s="2" t="n"/>
@@ -2599,12 +2599,12 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>MWK</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>Mexican Peso</t>
+          <t>Malawi Kwacha</t>
         </is>
       </c>
       <c r="C101" s="3" t="n"/>
@@ -2613,12 +2613,12 @@
     <row r="102">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MXV</t>
+          <t>MXN</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
         <is>
-          <t>Mexican Unidad de Inversion (UDI)</t>
+          <t>Mexican Peso</t>
         </is>
       </c>
       <c r="C102" s="2" t="n"/>
@@ -2627,12 +2627,12 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>MYR</t>
+          <t>MXV</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Malaysian Ringgit</t>
+          <t>Mexican Unidad de Inversion (UDI)</t>
         </is>
       </c>
       <c r="C103" s="3" t="n"/>
@@ -2641,12 +2641,12 @@
     <row r="104">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>MZN</t>
+          <t>MYR</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
         <is>
-          <t>Mozambique Metical</t>
+          <t>Malaysian Ringgit</t>
         </is>
       </c>
       <c r="C104" s="2" t="n"/>
@@ -2655,12 +2655,12 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>NAD</t>
+          <t>MZN</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>Namibia Dollar</t>
+          <t>Mozambique Metical</t>
         </is>
       </c>
       <c r="C105" s="3" t="n"/>
@@ -2669,12 +2669,12 @@
     <row r="106">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>NGN</t>
+          <t>NAD</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>Naira</t>
+          <t>Namibia Dollar</t>
         </is>
       </c>
       <c r="C106" s="2" t="n"/>
@@ -2683,12 +2683,12 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>NIO</t>
+          <t>NGN</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>Cordoba Oro</t>
+          <t>Naira</t>
         </is>
       </c>
       <c r="C107" s="3" t="n"/>
@@ -2697,12 +2697,12 @@
     <row r="108">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>NOK</t>
+          <t>NIO</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
         <is>
-          <t>Norwegian Krone</t>
+          <t>Cordoba Oro</t>
         </is>
       </c>
       <c r="C108" s="2" t="n"/>
@@ -2711,12 +2711,12 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>NPR</t>
+          <t>NOK</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>Nepalese Rupee</t>
+          <t>Norwegian Krone</t>
         </is>
       </c>
       <c r="C109" s="3" t="n"/>
@@ -2725,12 +2725,12 @@
     <row r="110">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>NZD</t>
+          <t>NPR</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
         <is>
-          <t>New Zealand Dollar</t>
+          <t>Nepalese Rupee</t>
         </is>
       </c>
       <c r="C110" s="2" t="n"/>
@@ -2739,12 +2739,12 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>OMR</t>
+          <t>NZD</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>Rial Omani</t>
+          <t>New Zealand Dollar</t>
         </is>
       </c>
       <c r="C111" s="3" t="n"/>
@@ -2753,12 +2753,12 @@
     <row r="112">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>PAB</t>
+          <t>OMR</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
         <is>
-          <t>Balboa</t>
+          <t>Rial Omani</t>
         </is>
       </c>
       <c r="C112" s="2" t="n"/>
@@ -2767,12 +2767,12 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>PEN</t>
+          <t>PAB</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>Sol</t>
+          <t>Balboa</t>
         </is>
       </c>
       <c r="C113" s="3" t="n"/>
@@ -2781,12 +2781,12 @@
     <row r="114">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>PGK</t>
+          <t>PEN</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
         <is>
-          <t>Kina</t>
+          <t>Sol</t>
         </is>
       </c>
       <c r="C114" s="2" t="n"/>
@@ -2795,12 +2795,12 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>PHP</t>
+          <t>PGK</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>Philippine Peso</t>
+          <t>Kina</t>
         </is>
       </c>
       <c r="C115" s="3" t="n"/>
@@ -2809,12 +2809,12 @@
     <row r="116">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>PKR</t>
+          <t>PHP</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
         <is>
-          <t>Pakistan Rupee</t>
+          <t>Philippine Peso</t>
         </is>
       </c>
       <c r="C116" s="2" t="n"/>
@@ -2823,12 +2823,12 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>PKR</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>Zloty</t>
+          <t>Pakistan Rupee</t>
         </is>
       </c>
       <c r="C117" s="3" t="n"/>
@@ -2837,12 +2837,12 @@
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>PYG</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Zloty</t>
         </is>
       </c>
       <c r="C118" s="2" t="n"/>
@@ -2851,12 +2851,12 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>QAR</t>
+          <t>PYG</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>Qatari Rial</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="C119" s="3" t="n"/>
@@ -2865,12 +2865,12 @@
     <row r="120">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>RON</t>
+          <t>QAR</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
         <is>
-          <t>Romanian Leu</t>
+          <t>Qatari Rial</t>
         </is>
       </c>
       <c r="C120" s="2" t="n"/>
@@ -2879,12 +2879,12 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>RSD</t>
+          <t>RON</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>Serbian Dinar</t>
+          <t>Romanian Leu</t>
         </is>
       </c>
       <c r="C121" s="3" t="n"/>
@@ -2893,12 +2893,12 @@
     <row r="122">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>RUB</t>
+          <t>RSD</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
         <is>
-          <t>Russian Ruble</t>
+          <t>Serbian Dinar</t>
         </is>
       </c>
       <c r="C122" s="2" t="n"/>
@@ -2907,12 +2907,12 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>RWF</t>
+          <t>RUB</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>Rwanda Franc</t>
+          <t>Russian Ruble</t>
         </is>
       </c>
       <c r="C123" s="3" t="n"/>
@@ -2921,12 +2921,12 @@
     <row r="124">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>SAR</t>
+          <t>RWF</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
         <is>
-          <t>Saudi Riyal</t>
+          <t>Rwanda Franc</t>
         </is>
       </c>
       <c r="C124" s="2" t="n"/>
@@ -2935,12 +2935,12 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>SBD</t>
+          <t>SAR</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>Solomon Islands Dollar</t>
+          <t>Saudi Riyal</t>
         </is>
       </c>
       <c r="C125" s="3" t="n"/>
@@ -2949,12 +2949,12 @@
     <row r="126">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>SCR</t>
+          <t>SBD</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
         <is>
-          <t>Seychelles Rupee</t>
+          <t>Solomon Islands Dollar</t>
         </is>
       </c>
       <c r="C126" s="2" t="n"/>
@@ -2963,12 +2963,12 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>SDG</t>
+          <t>SCR</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>Sudanese Pound</t>
+          <t>Seychelles Rupee</t>
         </is>
       </c>
       <c r="C127" s="3" t="n"/>
@@ -2977,12 +2977,12 @@
     <row r="128">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>SEK</t>
+          <t>SDG</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
         <is>
-          <t>Swedish Krona</t>
+          <t>Sudanese Pound</t>
         </is>
       </c>
       <c r="C128" s="2" t="n"/>
@@ -2991,12 +2991,12 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>SEK</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>Singapore Dollar</t>
+          <t>Swedish Krona</t>
         </is>
       </c>
       <c r="C129" s="3" t="n"/>
@@ -3005,12 +3005,12 @@
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>SHP</t>
+          <t>SGD</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
         <is>
-          <t>Saint Helena Pound</t>
+          <t>Singapore Dollar</t>
         </is>
       </c>
       <c r="C130" s="2" t="n"/>
@@ -3019,12 +3019,12 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>SLL</t>
+          <t>SHP</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>Leone</t>
+          <t>Saint Helena Pound</t>
         </is>
       </c>
       <c r="C131" s="3" t="n"/>
@@ -3033,12 +3033,12 @@
     <row r="132">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>SOS</t>
+          <t>SLL</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
         <is>
-          <t>Somali Shilling</t>
+          <t>Leone</t>
         </is>
       </c>
       <c r="C132" s="2" t="n"/>
@@ -3047,12 +3047,12 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>SRD</t>
+          <t>SOS</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>Surinam Dollar</t>
+          <t>Somali Shilling</t>
         </is>
       </c>
       <c r="C133" s="3" t="n"/>
@@ -3061,12 +3061,12 @@
     <row r="134">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>SSP</t>
+          <t>SRD</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
         <is>
-          <t>South Sudanese Pound</t>
+          <t>Surinam Dollar</t>
         </is>
       </c>
       <c r="C134" s="2" t="n"/>
@@ -3075,12 +3075,12 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>STN</t>
+          <t>SSP</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>Dobra</t>
+          <t>South Sudanese Pound</t>
         </is>
       </c>
       <c r="C135" s="3" t="n"/>
@@ -3089,12 +3089,12 @@
     <row r="136">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SVC</t>
+          <t>STN</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>El Salvador Colon</t>
+          <t>Dobra</t>
         </is>
       </c>
       <c r="C136" s="2" t="n"/>
@@ -3103,12 +3103,12 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>SYP</t>
+          <t>SVC</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>Syrian Pound</t>
+          <t>El Salvador Colon</t>
         </is>
       </c>
       <c r="C137" s="3" t="n"/>
@@ -3117,12 +3117,12 @@
     <row r="138">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>SZL</t>
+          <t>SYP</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>Lilangeni</t>
+          <t>Syrian Pound</t>
         </is>
       </c>
       <c r="C138" s="2" t="n"/>
@@ -3131,12 +3131,12 @@
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>THB</t>
+          <t>SZL</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>Baht</t>
+          <t>Lilangeni</t>
         </is>
       </c>
       <c r="C139" s="3" t="n"/>
@@ -3145,12 +3145,12 @@
     <row r="140">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>TJS</t>
+          <t>THB</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>Somoni</t>
+          <t>Baht</t>
         </is>
       </c>
       <c r="C140" s="2" t="n"/>
@@ -3159,12 +3159,12 @@
     <row r="141">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>TMT</t>
+          <t>TJS</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>Turkmenistan New Manat</t>
+          <t>Somoni</t>
         </is>
       </c>
       <c r="C141" s="3" t="n"/>
@@ -3173,12 +3173,12 @@
     <row r="142">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>TND</t>
+          <t>TMT</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>Tunisian Dinar</t>
+          <t>Turkmenistan New Manat</t>
         </is>
       </c>
       <c r="C142" s="2" t="n"/>
@@ -3187,12 +3187,12 @@
     <row r="143">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>TOP</t>
+          <t>TND</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>Pa’anga</t>
+          <t>Tunisian Dinar</t>
         </is>
       </c>
       <c r="C143" s="3" t="n"/>
@@ -3201,12 +3201,12 @@
     <row r="144">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>TRY</t>
+          <t>TOP</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>Turkish Lira</t>
+          <t>Pa’anga</t>
         </is>
       </c>
       <c r="C144" s="2" t="n"/>
@@ -3215,12 +3215,12 @@
     <row r="145">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>TTD</t>
+          <t>TRY</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago Dollar</t>
+          <t>Turkish Lira</t>
         </is>
       </c>
       <c r="C145" s="3" t="n"/>
@@ -3229,12 +3229,12 @@
     <row r="146">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>TWD</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
         <is>
-          <t>New Taiwan Dollar</t>
+          <t>Trinidad and Tobago Dollar</t>
         </is>
       </c>
       <c r="C146" s="2" t="n"/>
@@ -3243,12 +3243,12 @@
     <row r="147">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>TZS</t>
+          <t>TWD</t>
         </is>
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>Tanzanian Shilling</t>
+          <t>New Taiwan Dollar</t>
         </is>
       </c>
       <c r="C147" s="3" t="n"/>
@@ -3257,12 +3257,12 @@
     <row r="148">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>UAH</t>
+          <t>TZS</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
         <is>
-          <t>Hryvnia</t>
+          <t>Tanzanian Shilling</t>
         </is>
       </c>
       <c r="C148" s="2" t="n"/>
@@ -3271,12 +3271,12 @@
     <row r="149">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>UGX</t>
+          <t>UAH</t>
         </is>
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>Uganda Shilling</t>
+          <t>Hryvnia</t>
         </is>
       </c>
       <c r="C149" s="3" t="n"/>
@@ -3285,12 +3285,12 @@
     <row r="150">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>UGX</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
         <is>
-          <t>US Dollar</t>
+          <t>Uganda Shilling</t>
         </is>
       </c>
       <c r="C150" s="2" t="n"/>
@@ -3299,12 +3299,12 @@
     <row r="151">
       <c r="A151" s="3" t="inlineStr">
         <is>
-          <t>USN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>US Dollar (Next day)</t>
+          <t>US Dollar</t>
         </is>
       </c>
       <c r="C151" s="3" t="n"/>
@@ -3313,12 +3313,12 @@
     <row r="152">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>UYI</t>
+          <t>USN</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
         <is>
-          <t>Uruguay Peso en Unidades Indexadas (UI)</t>
+          <t>US Dollar (Next day)</t>
         </is>
       </c>
       <c r="C152" s="2" t="n"/>
@@ -3327,12 +3327,12 @@
     <row r="153">
       <c r="A153" s="3" t="inlineStr">
         <is>
-          <t>UYU</t>
+          <t>UYI</t>
         </is>
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>Peso Uruguayo</t>
+          <t>Uruguay Peso en Unidades Indexadas (UI)</t>
         </is>
       </c>
       <c r="C153" s="3" t="n"/>
@@ -3341,12 +3341,12 @@
     <row r="154">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>UYW</t>
+          <t>UYU</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
         <is>
-          <t>Unidad Previsional</t>
+          <t>Peso Uruguayo</t>
         </is>
       </c>
       <c r="C154" s="2" t="n"/>
@@ -3355,12 +3355,12 @@
     <row r="155">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>UZS</t>
+          <t>UYW</t>
         </is>
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>Uzbekistan Sum</t>
+          <t>Unidad Previsional</t>
         </is>
       </c>
       <c r="C155" s="3" t="n"/>
@@ -3369,12 +3369,12 @@
     <row r="156">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>VED</t>
+          <t>UZS</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
         <is>
-          <t>Bolívar Soberano</t>
+          <t>Uzbekistan Sum</t>
         </is>
       </c>
       <c r="C156" s="2" t="n"/>
@@ -3383,7 +3383,7 @@
     <row r="157">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>VES</t>
+          <t>VED</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -3397,12 +3397,12 @@
     <row r="158">
       <c r="A158" s="2" t="inlineStr">
         <is>
-          <t>VND</t>
+          <t>VES</t>
         </is>
       </c>
       <c r="B158" s="2" t="inlineStr">
         <is>
-          <t>Dong</t>
+          <t>Bolívar Soberano</t>
         </is>
       </c>
       <c r="C158" s="2" t="n"/>
@@ -3411,12 +3411,12 @@
     <row r="159">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>VUV</t>
+          <t>VND</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>Vatu</t>
+          <t>Dong</t>
         </is>
       </c>
       <c r="C159" s="3" t="n"/>
@@ -3425,12 +3425,12 @@
     <row r="160">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>WST</t>
+          <t>VUV</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
         <is>
-          <t>Tala</t>
+          <t>Vatu</t>
         </is>
       </c>
       <c r="C160" s="2" t="n"/>
@@ -3439,12 +3439,12 @@
     <row r="161">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>XAF</t>
+          <t>WST</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>CFA Franc BEAC</t>
+          <t>Tala</t>
         </is>
       </c>
       <c r="C161" s="3" t="n"/>
@@ -3453,12 +3453,12 @@
     <row r="162">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>XAG</t>
+          <t>XAF</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
         <is>
-          <t>Silver</t>
+          <t>CFA Franc BEAC</t>
         </is>
       </c>
       <c r="C162" s="2" t="n"/>
@@ -3467,12 +3467,12 @@
     <row r="163">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>XAU</t>
+          <t>XAG</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>Silver</t>
         </is>
       </c>
       <c r="C163" s="3" t="n"/>
@@ -3481,12 +3481,12 @@
     <row r="164">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>XBA</t>
+          <t>XAU</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
         <is>
-          <t>Bond Markets Unit European Composite Unit (EURCO)</t>
+          <t>Gold</t>
         </is>
       </c>
       <c r="C164" s="2" t="n"/>
@@ -3495,12 +3495,12 @@
     <row r="165">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>XBB</t>
+          <t>XBA</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>Bond Markets Unit European Monetary Unit (E.M.U.-6)</t>
+          <t>Bond Markets Unit European Composite Unit (EURCO)</t>
         </is>
       </c>
       <c r="C165" s="3" t="n"/>
@@ -3509,12 +3509,12 @@
     <row r="166">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>XBC</t>
+          <t>XBB</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
         <is>
-          <t>Bond Markets Unit European Unit of Account 9 (E.U.A.-9)</t>
+          <t>Bond Markets Unit European Monetary Unit (E.M.U.-6)</t>
         </is>
       </c>
       <c r="C166" s="2" t="n"/>
@@ -3523,12 +3523,12 @@
     <row r="167">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>XBD</t>
+          <t>XBC</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>Bond Markets Unit European Unit of Account 17 (E.U.A.-17)</t>
+          <t>Bond Markets Unit European Unit of Account 9 (E.U.A.-9)</t>
         </is>
       </c>
       <c r="C167" s="3" t="n"/>
@@ -3537,12 +3537,12 @@
     <row r="168">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>XCD</t>
+          <t>XBD</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
         <is>
-          <t>East Caribbean Dollar</t>
+          <t>Bond Markets Unit European Unit of Account 17 (E.U.A.-17)</t>
         </is>
       </c>
       <c r="C168" s="2" t="n"/>
@@ -3551,12 +3551,12 @@
     <row r="169">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>XDR</t>
+          <t>XCD</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>SDR (Special Drawing Right)</t>
+          <t>East Caribbean Dollar</t>
         </is>
       </c>
       <c r="C169" s="3" t="n"/>
@@ -3565,12 +3565,12 @@
     <row r="170">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>XOF</t>
+          <t>XDR</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
         <is>
-          <t>CFA Franc BCEAO</t>
+          <t>SDR (Special Drawing Right)</t>
         </is>
       </c>
       <c r="C170" s="2" t="n"/>
@@ -3579,12 +3579,12 @@
     <row r="171">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>XPD</t>
+          <t>XOF</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Palladium</t>
+          <t>CFA Franc BCEAO</t>
         </is>
       </c>
       <c r="C171" s="3" t="n"/>
@@ -3593,12 +3593,12 @@
     <row r="172">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>XPF</t>
+          <t>XPD</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
         <is>
-          <t>CFP Franc</t>
+          <t>Palladium</t>
         </is>
       </c>
       <c r="C172" s="2" t="n"/>
@@ -3607,12 +3607,12 @@
     <row r="173">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>XPT</t>
+          <t>XPF</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>Platinum</t>
+          <t>CFP Franc</t>
         </is>
       </c>
       <c r="C173" s="3" t="n"/>
@@ -3621,12 +3621,12 @@
     <row r="174">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>XSU</t>
+          <t>XPT</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
         <is>
-          <t>Sucre</t>
+          <t>Platinum</t>
         </is>
       </c>
       <c r="C174" s="2" t="n"/>
@@ -3635,12 +3635,12 @@
     <row r="175">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>XTS</t>
+          <t>XSU</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Codes specifically reserved for testing purposes</t>
+          <t>Sucre</t>
         </is>
       </c>
       <c r="C175" s="3" t="n"/>
@@ -3649,12 +3649,12 @@
     <row r="176">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>XUA</t>
+          <t>XTS</t>
         </is>
       </c>
       <c r="B176" s="2" t="inlineStr">
         <is>
-          <t>ADB Unit of Account</t>
+          <t>Codes specifically reserved for testing purposes</t>
         </is>
       </c>
       <c r="C176" s="2" t="n"/>
@@ -3663,12 +3663,12 @@
     <row r="177">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>XUA</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>The codes assigned for transactions where no currency is involved</t>
+          <t>ADB Unit of Account</t>
         </is>
       </c>
       <c r="C177" s="3" t="n"/>
@@ -3677,12 +3677,12 @@
     <row r="178">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>YER</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
         <is>
-          <t>Yemeni Rial</t>
+          <t>The codes assigned for transactions where no currency is involved</t>
         </is>
       </c>
       <c r="C178" s="2" t="n"/>
@@ -3691,12 +3691,12 @@
     <row r="179">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>ZAR</t>
+          <t>YER</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>Rand</t>
+          <t>Yemeni Rial</t>
         </is>
       </c>
       <c r="C179" s="3" t="n"/>
@@ -3705,12 +3705,12 @@
     <row r="180">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>ZMW</t>
+          <t>ZAR</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
         <is>
-          <t>Zambian Kwacha</t>
+          <t>Rand</t>
         </is>
       </c>
       <c r="C180" s="2" t="n"/>
@@ -3719,16 +3719,30 @@
     <row r="181">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>ZWL</t>
+          <t>ZMW</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>Zimbabwe Dollar</t>
+          <t>Zambian Kwacha</t>
         </is>
       </c>
       <c r="C181" s="3" t="n"/>
       <c r="D181" s="3" t="n"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="inlineStr">
+        <is>
+          <t>ZWL</t>
+        </is>
+      </c>
+      <c r="B182" s="2" t="inlineStr">
+        <is>
+          <t>Zimbabwe Dollar</t>
+        </is>
+      </c>
+      <c r="C182" s="2" t="n"/>
+      <c r="D182" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
New codelists from release RC10 and RC11
</commit_message>
<xml_diff>
--- a/Codelists/Codelists - Import.xlsx
+++ b/Codelists/Codelists - Import.xlsx
@@ -18,39 +18,42 @@
     <sheet name="10035" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="10038" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="10057" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="10146" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="10171" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="10175" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="10183" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="10187" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="10203" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="10209" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="10213" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="10214" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="10218" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="10223" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="10226" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="10227" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="10230" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="10234" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="10236" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="10238" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="10239" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="10240" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="10242" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="10243" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="10250" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="10268" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="10272" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="10273" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="10274" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="10275" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="10276" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="10282" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="11000" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="11034" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="11038" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="50001" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="10066" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="10146" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="10171" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="10175" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="10183" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="10187" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="10203" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="10209" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="10213" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="10214" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="10218" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="10223" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="10226" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="10227" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="10230" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="10234" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="10236" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="10238" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="10239" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="10240" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="10242" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="10243" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="10250" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="10268" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="10272" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="10273" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="10274" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="10275" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="10276" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="10282" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="11000" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="11034" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="11038" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="11068" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="11082" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="50001" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -900,7 +903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -932,7 +935,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Corrected  by Customs</t>
+          <t>Corrected by Customs (No Risk Assessment)</t>
         </is>
       </c>
       <c r="C2" s="2" t="n"/>
@@ -955,12 +958,12 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Corrected - by DMS</t>
+          <t>Corrected by Customs (Risk Assessment)</t>
         </is>
       </c>
       <c r="C4" s="2" t="n"/>
@@ -969,12 +972,12 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Partial invalidation</t>
+          <t>Corrected - by DMS</t>
         </is>
       </c>
       <c r="C5" s="3" t="n"/>
@@ -983,12 +986,12 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM 22 Goods, which has been sold under a distance contract and have been released for free circulation, have been returned</t>
+          <t>Partial invalidation</t>
         </is>
       </c>
       <c r="C6" s="2" t="n"/>
@@ -997,12 +1000,12 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM EX TR 23 Where union goods have been declared in error for a customs procedure applicable to non-union goods, and their customs status as union goods have been proved afterwards by means of a T2L, T2LF or a customs goods manifest</t>
+          <t>Partial invalidation - IM 22 Goods, which has been sold under a distance contract and have been released for free circulation, have been returned</t>
         </is>
       </c>
       <c r="C7" s="3" t="n"/>
@@ -1011,12 +1014,12 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM EX TR 24 Where goods have been erroneously declared under more than one customs declaration</t>
+          <t>Partial invalidation - IM EX TR 23 Where union goods have been declared in error for a customs procedure applicable to non-union goods, and their customs status as union goods have been proved afterwards by means of a T2L, T2LF or a customs goods manifest</t>
         </is>
       </c>
       <c r="C8" s="2" t="n"/>
@@ -1025,12 +1028,12 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM 25 Postal low value consignments returned on basis of barcode S10</t>
+          <t>Partial invalidation - IM EX TR 24 Where goods have been erroneously declared under more than one customs declaration</t>
         </is>
       </c>
       <c r="C9" s="3" t="n"/>
@@ -1039,12 +1042,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM EX TR 26 Accepted declaration with goods to be placed under another customs procedure</t>
+          <t>Partial invalidation - IM 25 Postal low value consignments returned on basis of barcode S10</t>
         </is>
       </c>
       <c r="C10" s="2" t="n"/>
@@ -1053,12 +1056,12 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM 27 Accepted declaration where the customs procedure is no longer justified due to special circumstances</t>
+          <t>Partial invalidation - IM EX TR 26 Accepted declaration with goods to be placed under another customs procedure</t>
         </is>
       </c>
       <c r="C11" s="3" t="n"/>
@@ -1067,12 +1070,12 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM EX TR 28 Where goods to be destroyed, abandoned to the State, seized or confiscated are already subject to a customs declaration.</t>
+          <t>Partial invalidation - IM 27 Accepted declaration where the customs procedure is no longer justified due to special circumstances</t>
         </is>
       </c>
       <c r="C12" s="2" t="n"/>
@@ -1081,12 +1084,12 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM 29 Goods declared in error to a customs procedure incurring a customs debt</t>
+          <t>Partial invalidation - IM EX TR 28 Where goods to be destroyed, abandoned to the State, seized or confiscated are already subject to a customs declaration.</t>
         </is>
       </c>
       <c r="C13" s="3" t="n"/>
@@ -1095,12 +1098,12 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM 30 Goods declared in error instead of other goods incurring a customs debt</t>
+          <t>Partial invalidation - IM 29 Goods declared in error to a customs procedure incurring a customs debt</t>
         </is>
       </c>
       <c r="C14" s="2" t="n"/>
@@ -1109,12 +1112,12 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Partial invalidation - IM EX 31 Where an authorization with retroactive effect is granted in accordance with Article 211(2) of the Code</t>
+          <t>Partial invalidation - IM 30 Goods declared in error instead of other goods incurring a customs debt</t>
         </is>
       </c>
       <c r="C15" s="3" t="n"/>
@@ -1123,12 +1126,12 @@
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>Corrected by declarant</t>
+          <t>Partial invalidation - IM EX 31 Where an authorization with retroactive effect is granted in accordance with Article 211(2) of the Code</t>
         </is>
       </c>
       <c r="C16" s="2" t="n"/>
@@ -1137,12 +1140,12 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Addition of missing data element (obsolete- no longer needed)</t>
+          <t>Corrected by declarant</t>
         </is>
       </c>
       <c r="C17" s="3" t="n"/>
@@ -1151,12 +1154,12 @@
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>Mistaken Customs Procedure</t>
+          <t>Addition of missing data element (obsolete- no longer needed)</t>
         </is>
       </c>
       <c r="C18" s="2" t="n"/>
@@ -1165,16 +1168,30 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Special circumstances that do not justify placement</t>
+          <t>Mistaken Customs Procedure</t>
         </is>
       </c>
       <c r="C19" s="3" t="n"/>
       <c r="D19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Special circumstances that do not justify placement</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1182,6 +1199,335 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>IM 122 - Goods, which have been sold under a distance contract and have been released for free circulation, have been returned</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 123 - Where union goods have been declared in error for a customs procedure applicable to non-union goods, and their customs status as union goods have been proved afterwards by means of a T2L, T2LF or a customs goods manifest</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 124 - Where goods have been erroneously declared under more than one customs declaration</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>IM 125 - Postal low value consignments returned on basis of barcode S10</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 126 - Accepted declaration with goods to be placed under another customs procedure</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>IM 127 - Accepted declaration where the customs procedure is no longer justified due to special circumstances</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 128 - Where goods to be destroyed, abandoned to the State, seized or confiscated are already subject to a customs declaration</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>IM 129 - Goods declared in error to a customs procedure incurring a customs debt</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>IM 130 - Goods declared in error instead of other goods incurring a customs debt</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>IM, EX 131 - Where an authorization with retroactive effect is granted in accordance with Article 211(2) of the Code</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>EX 132 - Where the discrepancy in the nature of the goods released for export, re-export or outward processing compared to those presented to the customs office of exit, the customs office of export, shall invalidate the declaration concerned</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>EX 133 - Where, after a period of 150 days from the date of release of the goods, the customs office of export has received neither information on the exit of the goods nor evidence that the goods have left the customs territory of the Union</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>EX 134 - The declarant informs the customs office of export, that the goods released for export, re-export or outwards processing, will not leave the Union</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>EX 135 - Where union goods have been placed under the customs warehousing procedure in accordance with article 237(2) of the code and can no longer be placed under that procedure in accordance with article 237(2) of the code</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>136</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>EX 136 - The customs office of export has been informed that the goods were not taken out of the territory of the Union</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>EX 138 - Goods for which an exit summary declaration has been lodged, which have not yet left the Union</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>EX 139 - Goods for which a re-export notification has been lodged, which have not yet left the Union</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>EX 141 - Where the goods for which an exit summary declaration has been lodged are not taken out of the customs territory of the Union within 150 days after the lodging of the declaration</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>EX 142 - Where the goods for which a re-export notification has been lodged are not taken out of the customs territory of the Union within 150 days after the lodging of the declaration</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>IM 145 Invalidation of declaration for temperary storage, where the goods has not yet been presented to the customs authorities, upon application by the declarant</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n"/>
+      <c r="D21" s="3" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>IM 146 Invalidation of declaration for temperory storage, where the goods has not yet been presented to the customs authorities 30 days after the declaration was lodged</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1636,7 +1982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4191,7 +4537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4416,181 +4762,6 @@
       </c>
       <c r="C15" s="3" t="n"/>
       <c r="D15" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>BOD</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Bill Of Discharge</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>BULK_GPR</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Bulk GPR</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>COR</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Request Correction/Amendment</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>GPR</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Notify Goods Presentation</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>I2GPR</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Present Goods via I2 declaration</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>INV</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Request Invalidation</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>INV4C</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Request Invalidation &amp; Remission (4c)</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>RDG</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>Request for Disposal of Goods</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="3" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>RRA</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Repayment/Remission 4c</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>SUP</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>Supplementary declaration after incomplete</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4630,12 +4801,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>IM 122 - Goods, which have been sold under a distance contract and have been released for free circulation, have been returned</t>
+          <t>Bill Of Discharge</t>
         </is>
       </c>
       <c r="C2" s="2" t="n"/>
@@ -4644,12 +4815,12 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>BULK_GPR</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>IM, EX, TR 123 - Where union goods have been declared in error for a customs procedure applicable to non-union goods, and their customs status as union goods have been proved afterwards by means of a T2L, T2LF or a customs goods manifest</t>
+          <t>Bulk GPR</t>
         </is>
       </c>
       <c r="C3" s="3" t="n"/>
@@ -4658,12 +4829,12 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>IM, EX, TR 124 - Where goods have been erroneously declared under more than one customs declaration</t>
+          <t>Request Correction/Amendment</t>
         </is>
       </c>
       <c r="C4" s="2" t="n"/>
@@ -4672,12 +4843,12 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>GPR</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>IM 125 - Postal low value consignments returned on basis of barcode S10</t>
+          <t>Notify Goods Presentation</t>
         </is>
       </c>
       <c r="C5" s="3" t="n"/>
@@ -4686,12 +4857,12 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>I2GPR</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>IM, EX, TR 126 - Accepted declaration with goods to be placed under another customs procedure</t>
+          <t>Present Goods via I2 declaration</t>
         </is>
       </c>
       <c r="C6" s="2" t="n"/>
@@ -4700,12 +4871,12 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>INV</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>IM 127 - Accepted declaration where the customs procedure is no longer justified due to special circumstances</t>
+          <t>Request Invalidation</t>
         </is>
       </c>
       <c r="C7" s="3" t="n"/>
@@ -4714,12 +4885,12 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>INV4C</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>IM 129 - Goods declared in error to a customs procedure incurring a customs debt</t>
+          <t>Request Invalidation &amp; Remission (4c)</t>
         </is>
       </c>
       <c r="C8" s="2" t="n"/>
@@ -4728,12 +4899,12 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>RDG</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>IM 130 - Goods declared in error instead of other goods incurring a customs debt</t>
+          <t>Request for Disposal of Goods</t>
         </is>
       </c>
       <c r="C9" s="3" t="n"/>
@@ -4742,12 +4913,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>RRA</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>IM, EX 131 - Where an authorization with retroactive effect is granted in accordance with Article 211(2) of the Code</t>
+          <t>Repayment/Remission 4c</t>
         </is>
       </c>
       <c r="C10" s="2" t="n"/>
@@ -4756,12 +4927,12 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>SUP</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>IM 145 Invalidation of declaration for temperary storage, where the goods has not yet been presented to the customs authorities, upon application by the declarant</t>
+          <t>Supplementary declaration after incomplete</t>
         </is>
       </c>
       <c r="C11" s="3" t="n"/>
@@ -4773,6 +4944,237 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>IM 122 - Goods, which have been sold under a distance contract and have been released for free circulation, have been returned</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 123 - Where union goods have been declared in error for a customs procedure applicable to non-union goods, and their customs status as union goods have been proved afterwards by means of a T2L, T2LF or a customs goods manifest</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 124 - Where goods have been erroneously declared under more than one customs declaration</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>IM 125 - Postal low value consignments returned on basis of barcode S10</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>IM, EX, TR 126 - Accepted declaration with goods to be placed under another customs procedure</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>IM 127 - Accepted declaration where the customs procedure is no longer justified due to special circumstances</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>IM 129 - Goods declared in error to a customs procedure incurring a customs debt</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>IM 130 - Goods declared in error instead of other goods incurring a customs debt</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>IM, EX 131 - Where an authorization with retroactive effect is granted in accordance with Article 211(2) of the Code</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>EX 134 - The declarant informs the customs office of export, that the goods released for export, re-export or outwards processing, will not leave the Union</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>EX 135 - Where union goods have been placed under the customs warehousing procedure in accordance with article 237(2) of the code and can no longer be placed under that procedure in accordance with article 237(2) of the code</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>EX 138 - Goods for which an exit summary declaration has been lodged, which have not yet left the Union</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>EX 139 - Goods for which a re-export notification has been lodged, which have not yet left the Union</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>IM 145 Invalidation of declaration for temperary storage, where the goods has not yet been presented to the customs authorities, upon application by the declarant</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8335,7 +8737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9120,139 +9522,6 @@
       </c>
       <c r="C55" s="3" t="n"/>
       <c r="D55" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Public customs warehouse type I</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Public customs warehouse type II</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Public customs warehouse type III</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Private customs warehouse</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Storage facilities for the temporary storage of goods</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Non-customs warehouse</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Free zone</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10235,7 +10504,7 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>pct</t>
+          <t>%</t>
         </is>
       </c>
       <c r="C69" s="3" t="n"/>
@@ -10415,6 +10684,139 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Public customs warehouse type I</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Public customs warehouse type II</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Public customs warehouse type III</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>U</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Private customs warehouse</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Storage facilities for the temporary storage of goods</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Non-customs warehouse</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Free zone</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10603,7 +11005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -11548,7 +11950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -11975,7 +12377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -12192,7 +12594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -12269,7 +12671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -12906,7 +13308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -13389,7 +13791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -17260,7 +17662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -17429,125 +17831,6 @@
       </c>
       <c r="C11" s="3" t="n"/>
       <c r="D11" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>UN/LOCODE</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Customs office identifier</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>GPS coordinates</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>EORI number</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Authorisation number</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -23279,6 +23562,125 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>U</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>UN/LOCODE</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Customs office identifier</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>GPS coordinates</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>EORI number</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Authorisation number</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23364,7 +23766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -23637,7 +24039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -23728,7 +24130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -23847,7 +24249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -25296,7 +25698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -30273,7 +30675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -30826,7 +31228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -31323,7 +31725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -39590,349 +39992,6 @@
       </c>
       <c r="C589" s="3" t="n"/>
       <c r="D589" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>C613</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Consignment Note CIM T2</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>C614</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Consignment Note CIM T2F</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>N235</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Container list</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>N270</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Delivery Note</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>N271</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Packing list</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>N325</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Proforma invoice</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>N380</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Commercial invoice</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>N703</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>House waybill</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="3" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>N704</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Master bill of lading</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>N705</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>Bill of lading</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>N710</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>Bill of lading (T1)</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>N714</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>House bill of lading</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="n"/>
-      <c r="D13" s="3" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>N720</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>Consignment note CIM</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>N722</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>Road list - SMGS</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="n"/>
-      <c r="D15" s="3" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>N730</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>Road consignment note</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>N740</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="inlineStr">
-        <is>
-          <t>Air waybill</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="n"/>
-      <c r="D17" s="3" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>N741</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>Master airwaybill</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="n"/>
-      <c r="D18" s="2" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="inlineStr">
-        <is>
-          <t>N750</t>
-        </is>
-      </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>Movement by post including parcel post</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="n"/>
-      <c r="D19" s="3" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>N760</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>Multimodal / combined transport document</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="n"/>
-      <c r="D20" s="2" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>N785</t>
-        </is>
-      </c>
-      <c r="B21" s="3" t="inlineStr">
-        <is>
-          <t>Cargo manifest</t>
-        </is>
-      </c>
-      <c r="C21" s="3" t="n"/>
-      <c r="D21" s="3" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>N787</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Bordereau (cargo load list)</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="n"/>
-      <c r="D22" s="2" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>N955</t>
-        </is>
-      </c>
-      <c r="B23" s="3" t="inlineStr">
-        <is>
-          <t>ATA carnet</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="n"/>
-      <c r="D23" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -40008,6 +40067,349 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>C613</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Consignment Note CIM T2</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>C614</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Consignment Note CIM T2F</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>N235</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Container list</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>N270</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Delivery Note</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>N271</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Packing list</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>N325</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Proforma invoice</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>N380</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Commercial invoice</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>N703</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>House waybill</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>N704</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Master bill of lading</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>N705</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Bill of lading</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>N710</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Bill of lading (T1)</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>N714</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>House bill of lading</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>N720</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Consignment note CIM</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>N722</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Road list - SMGS</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>N730</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Road consignment note</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>N740</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Air waybill</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>N741</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>Master airwaybill</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>N750</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Movement by post including parcel post</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>N760</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Multimodal / combined transport document</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>N785</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Cargo manifest</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n"/>
+      <c r="D21" s="3" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>N787</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>Bordereau (cargo load list)</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>N955</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>ATA carnet</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -40051,7 +40453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -40590,7 +40992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -40933,7 +41335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -41010,7 +41412,735 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>C057</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Copy of the declaration of conformity - Option A, as referred to in Article 1.2 and in the Annex to Commission Implementing Regulation (EU) 2016/879</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>C079</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Copy of the declaration of conformity - Option B, as referred to in Article 1.2 and in the Annex to Commission Implementing Regulation (EU) 2016/879</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>C082</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Copy of the declaration of conformity - Option C, as referred to in Article 1.2 and in the Annex to Commission Implementing Regulation (EU) 2016/879</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>C085</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>CHED-PP - Common Health Entry Document for Plants and Plant Products</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>C400</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Presentation of the required 'CITES' certificate</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>C402</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>CITES Export permit or Re-export certificate issued by a third country</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>C638</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>CITES Import permit</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>C640</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>CHED-A - Common Health Entry Document for Animals</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>C644</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>COI - Certificate of inspection for organic products</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>C646</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>NOA - Notification of Arrival (Common Health Entry Document for Food and Feed of Non-Animal Origin, Food Contact Materials and Plant Protection Products)</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>C678</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>CHED-D - Common Health Entry Document for Feed and Food of Non-Animal Origin</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>C690</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>FLEGT - Forest Law Enforcement, Governance and Trade</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>E013</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>ODS Export - Export license "controlled substances" (ozone), issued by the Commission</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>L049</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>ICGL - Import licence for cultural goods, issued in accordance with Article 4 of Regulation (EU) 2019/880</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>L050</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>ICGS - Importer statement for cultural goods (Article 5 of Regulation (EU) 2019/880)</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>L065</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>ICGS - Importer statement for cultural goods, presented in lieu of a licence, for cultural goods that have been placed under the temporary admission procedure (Article 3.5 of Regulation (EU) 2019/880)</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>L100</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>ODS Import - Import license "controlled substances" (ozone), issued by the Commission</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>N853</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>CHED-P - Common Health Entry Document for Animal Products</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>X060</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>DUES Individual Export Authorisation - Article 12(1)(a) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>X061</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU001 - ANNEX II A - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n"/>
+      <c r="D21" s="3" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>X062</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU002 - ANNEX II B - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>X063</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU003 - ANNEX II C - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" s="3" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>X064</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU004 - ANNEX II D - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>X065</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU005 - ANNEX II E - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="n"/>
+      <c r="D25" s="3" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>X066</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU006 - ANNEX II F - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>X067</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU007 - ANNEX II G - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n"/>
+      <c r="D27" s="3" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>X068</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>DUES Union General Export Authorisation No EU008 - ANNEX II H - referred to in Article 12(1)(d) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>X070</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>DUES Global Export Authorisation - referred to in Article 12(1)(b) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n"/>
+      <c r="D29" s="3" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>X071</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>DUES National General Export Authorisations in national Official Journals - ANNEX III C - referred to in Article 12(6) of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>X072</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>DUES Transit Licence for dual Use Items - referred to in Article 7 of the Regulation (EU) 2021/821 of the European Parliament and of the Council</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n"/>
+      <c r="D31" s="3" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Y120</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Undertaking importing less than 100 tonnes of CO2 equivalent of hydrofluorocarbons per year and exempted from the reduction of the quantity of hydrofluorocarbons placed on the EU market according to article 15.2 first sub paragraph</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n"/>
+      <c r="D32" s="2" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>Y123</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>FGAS - Undertaking registered in the F-Gas Portal according to Article 20 of Regulation (EU) 2024/573/573</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="n"/>
+      <c r="D33" s="3" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Y124</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Undertaking importing smaller amount of fluorinated greenhouse gases per year than that specified in Article 19.1 for bulk imports and 19.4 for products and equipment imports, and therefore not covered by the registration requirement</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n"/>
+      <c r="D34" s="2" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>Y125</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>Import falling under Article 15.1 of Regulation (EU) N° 517/2014 on the reduction of the quantity of hydrofluorocarbons placed on the EU market</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n"/>
+      <c r="D35" s="3" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Y128</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>CBAM - Unique Account Number of the Authorised CBAM Declarant, in accordance with Article 16.1 of Regulation (EU) 2023/956</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>Y139</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>ICGD - Derogation for goods imported as per Article 3.4(b) and (c) of Regulation (EU) 2019/880</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n"/>
+      <c r="D37" s="3" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Y152</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>FGAS - Exemption from import prohibition, granted for repair or servicing of existing equipment, according to the second paragraph of Article 11.1 of Regulation (EU) 2024/573</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n"/>
+      <c r="D38" s="2" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>Y154</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>FGAS - Exemption from import/export prohibition on containers, non-refillable or without refilling provisions, for fluorinated greenhouse gases, empty or fully or partially filled, for laboratory or analytical uses according to Art.11.3 Reg. 2024/573</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n"/>
+      <c r="D39" s="3" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Y161</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>FGAS - Exemption from export prohibition according to Article 22.3, second subparagraph of Regulation (EU) 2024/573</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="2" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>Y951</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>Exemption from the reduction of the quantity of hydrofluorocarbons placed on the market by virtue of Article 15.2 (a) to (f) of Regulation (EU) No 517/2014</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="n"/>
+      <c r="D41" s="3" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>Y972</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>FGAS - Exemption from the reduction of the quantity of hydrofluorocarbons placed on the market by virtue of Article 16.2 (c) of Regulation (EU) 2024/573</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n"/>
+      <c r="D42" s="2" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>Y986</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>Exemption from import prohibition according to Article 11.1 and 11.2 of Regulation (EU) N° 517/2014</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="n"/>
+      <c r="D43" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Y121</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>FGAS Tones of CO2 equivalent of bulk gases and of gases contained in products or equipment, and parts thereof</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Y163</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>FGAS Net mass of F-gases charged in products and equipment</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Y797</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>ODS - Licensing system registration identification number as defined in Article 17.3 (a)</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Y798</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>ODS - Declaration of net mass of ozone -depleting substance(s), when included in products and equipment</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Y799</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>ODS - net mass of the ODS multiplied by the ODP of the ozone-depleting substance(s), also when included in products and equipment</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>